<commit_message>
updated files from tufts
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
+++ b/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
@@ -362,7 +362,7 @@
     <xdr:ext cx="8048625" cy="4362450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -390,7 +390,7 @@
     <xdr:ext cx="8229600" cy="4362450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
updated files from tufts 5/14
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
+++ b/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
@@ -362,7 +362,7 @@
     <xdr:ext cx="8048625" cy="4362450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -390,7 +390,7 @@
     <xdr:ext cx="8229600" cy="4362450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
updated files from tufts 5/28
</commit_message>
<xml_diff>
--- a/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
+++ b/InputData/elec/BHRbEF/BAU Heat Rate by Electricity Fuel.xlsx
@@ -362,7 +362,7 @@
     <xdr:ext cx="8048625" cy="4362450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -390,7 +390,7 @@
     <xdr:ext cx="8229600" cy="4362450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>